<commit_message>
Added aiden's changes and formatted csv
</commit_message>
<xml_diff>
--- a/xpod_node/header.xlsx
+++ b/xpod_node/header.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\being\OneDrive\Desktop\git\xpod\xpod_node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C618A15-D99D-4192-A39A-1AC0FE156E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D0DB79-48A4-4AC1-81BC-1EC5054D3B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{66BEC1FB-651A-4226-BA1D-34D28E7FC29E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>DateTime</t>
   </si>
@@ -53,9 +53,6 @@
     <t>FIG 3 (raw)</t>
   </si>
   <si>
-    <t>FIG 4 (raw)</t>
-  </si>
-  <si>
     <t>PID</t>
   </si>
   <si>
@@ -156,6 +153,75 @@
   </si>
   <si>
     <t>wind_dir</t>
+  </si>
+  <si>
+    <t>(YYYY-MM-DDThh:mm:ss)</t>
+  </si>
+  <si>
+    <t>Raw Sensor value</t>
+  </si>
+  <si>
+    <t>Raw Sensor Value</t>
+  </si>
+  <si>
+    <t>Raw Heater Value</t>
+  </si>
+  <si>
+    <t>Figaro 4 (raw)</t>
+  </si>
+  <si>
+    <t>Figaro 3(Heater)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figaro 4(Heater) </t>
+  </si>
+  <si>
+    <t>(in volts)</t>
+  </si>
+  <si>
+    <t>In degree C</t>
+  </si>
+  <si>
+    <t>hpa</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Raw Val</t>
+  </si>
+  <si>
+    <t>Quad 1 Channel 1</t>
+  </si>
+  <si>
+    <t>Quad 1 Channel 2</t>
+  </si>
+  <si>
+    <t>Quad 1 Channel 3</t>
+  </si>
+  <si>
+    <t>Quad 1 Channel 4</t>
+  </si>
+  <si>
+    <t>Quad 2 Channel 1</t>
+  </si>
+  <si>
+    <t>Quad 2 Channel 2</t>
+  </si>
+  <si>
+    <t>Quad 2 Channel 3</t>
+  </si>
+  <si>
+    <t>Quad 2 Channel 4</t>
+  </si>
+  <si>
+    <t>Raw Value</t>
+  </si>
+  <si>
+    <t>Gps date</t>
+  </si>
+  <si>
+    <t>GPS time</t>
   </si>
 </sst>
 </file>
@@ -507,32 +573,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDB920D-B1A9-4387-A7B5-1A029C405504}">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" customWidth="1"/>
-    <col min="24" max="24" width="11" customWidth="1"/>
-    <col min="25" max="26" width="9.77734375" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" customWidth="1"/>
-    <col min="36" max="36" width="10.77734375" customWidth="1"/>
-    <col min="39" max="39" width="12" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.77734375" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" customWidth="1"/>
+    <col min="20" max="20" width="17.21875" customWidth="1"/>
+    <col min="21" max="21" width="16.77734375" customWidth="1"/>
+    <col min="22" max="22" width="16.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.88671875" customWidth="1"/>
+    <col min="26" max="27" width="9.77734375" customWidth="1"/>
+    <col min="28" max="28" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.33203125" customWidth="1"/>
+    <col min="37" max="37" width="10.77734375" customWidth="1"/>
+    <col min="38" max="38" width="10.6640625" customWidth="1"/>
+    <col min="40" max="40" width="12" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,112 +627,196 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+    </row>
+    <row r="2" spans="1:42" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>